<commit_message>
merged to brady's branch
</commit_message>
<xml_diff>
--- a/Optimization_Stats.xlsx
+++ b/Optimization_Stats.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
   <si>
     <t>Schedule (Pre-Optimization)</t>
   </si>
@@ -80,12 +80,12 @@
     <t>Division U9 (Tier: 0)</t>
   </si>
   <si>
+    <t>72.73%</t>
+  </si>
+  <si>
     <t>Division U9 (Tier: 1)</t>
   </si>
   <si>
-    <t>72.73%</t>
-  </si>
-  <si>
     <t>Division U9 (Tier: 2)</t>
   </si>
   <si>
@@ -98,16 +98,22 @@
     <t>Schedule (Post-Optimization)</t>
   </si>
   <si>
+    <t>86.36%</t>
+  </si>
+  <si>
+    <t>87.5%</t>
+  </si>
+  <si>
+    <t>100.0%</t>
+  </si>
+  <si>
+    <t>97.73%</t>
+  </si>
+  <si>
     <t>84.09%</t>
   </si>
   <si>
-    <t>87.5%</t>
-  </si>
-  <si>
-    <t>100.0%</t>
-  </si>
-  <si>
-    <t>84.85%</t>
+    <t>85.61%</t>
   </si>
 </sst>
 </file>
@@ -400,27 +406,27 @@
         <v>22.0</v>
       </c>
       <c r="C9" t="n" s="1">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="D9" t="n" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="E9" t="n" s="1">
         <v>22.0</v>
       </c>
       <c r="F9" t="n" s="1">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="G9" t="n" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="H9" t="s" s="1">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" t="n" s="1">
         <v>44.0</v>
@@ -441,7 +447,7 @@
         <v>12.0</v>
       </c>
       <c r="H10" t="s" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
@@ -467,7 +473,7 @@
         <v>12.0</v>
       </c>
       <c r="H11" t="s" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
@@ -530,19 +536,19 @@
         <v>44.0</v>
       </c>
       <c r="C16" t="n" s="1">
-        <v>37.0</v>
+        <v>38.0</v>
       </c>
       <c r="D16" t="n" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="E16" t="n" s="1">
         <v>44.0</v>
       </c>
       <c r="F16" t="n" s="1">
-        <v>36.0</v>
+        <v>35.0</v>
       </c>
       <c r="G16" t="n" s="1">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="H16" t="s" s="1">
         <v>28</v>
@@ -556,10 +562,10 @@
         <v>44.0</v>
       </c>
       <c r="C17" t="n" s="1">
-        <v>37.0</v>
+        <v>36.0</v>
       </c>
       <c r="D17" t="n" s="1">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="E17" t="n" s="1">
         <v>44.0</v>
@@ -571,7 +577,7 @@
         <v>9.0</v>
       </c>
       <c r="H17" t="s" s="1">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18">
@@ -617,10 +623,10 @@
         <v>22.0</v>
       </c>
       <c r="F19" t="n" s="1">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="G19" t="n" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="H19" t="s" s="1">
         <v>30</v>
@@ -643,10 +649,10 @@
         <v>22.0</v>
       </c>
       <c r="F20" t="n" s="1">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="G20" t="n" s="1">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="H20" t="s" s="1">
         <v>30</v>
@@ -669,10 +675,10 @@
         <v>44.0</v>
       </c>
       <c r="F21" t="n" s="1">
-        <v>34.0</v>
+        <v>36.0</v>
       </c>
       <c r="G21" t="n" s="1">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="H21" t="s" s="1">
         <v>30</v>
@@ -686,22 +692,22 @@
         <v>44.0</v>
       </c>
       <c r="C22" t="n" s="1">
-        <v>44.0</v>
+        <v>43.0</v>
       </c>
       <c r="D22" t="n" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E22" t="n" s="1">
         <v>44.0</v>
       </c>
       <c r="F22" t="n" s="1">
-        <v>35.0</v>
+        <v>37.0</v>
       </c>
       <c r="G22" t="n" s="1">
-        <v>9.0</v>
+        <v>7.0</v>
       </c>
       <c r="H22" t="s" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23">
@@ -721,10 +727,10 @@
         <v>22.0</v>
       </c>
       <c r="F23" t="n" s="1">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="G23" t="n" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="H23" t="s" s="1">
         <v>12</v>
@@ -732,7 +738,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" t="n" s="1">
         <v>44.0</v>
@@ -747,10 +753,10 @@
         <v>44.0</v>
       </c>
       <c r="F24" t="n" s="1">
-        <v>33.0</v>
+        <v>35.0</v>
       </c>
       <c r="G24" t="n" s="1">
-        <v>11.0</v>
+        <v>9.0</v>
       </c>
       <c r="H24" t="s" s="1">
         <v>30</v>
@@ -764,10 +770,10 @@
         <v>44.0</v>
       </c>
       <c r="C25" t="n" s="1">
-        <v>36.0</v>
+        <v>37.0</v>
       </c>
       <c r="D25" t="n" s="1">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="E25" t="n" s="1">
         <v>44.0</v>
@@ -779,7 +785,7 @@
         <v>10.0</v>
       </c>
       <c r="H25" t="s" s="1">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26">
@@ -790,22 +796,22 @@
         <v>132.0</v>
       </c>
       <c r="C26" t="n" s="1">
-        <v>112.0</v>
+        <v>113.0</v>
       </c>
       <c r="D26" t="n" s="1">
-        <v>20.0</v>
+        <v>19.0</v>
       </c>
       <c r="E26" t="n" s="1">
         <v>132.0</v>
       </c>
       <c r="F26" t="n" s="1">
-        <v>97.0</v>
+        <v>94.0</v>
       </c>
       <c r="G26" t="n" s="1">
-        <v>35.0</v>
+        <v>38.0</v>
       </c>
       <c r="H26" t="s" s="1">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added TabuSearch_Stats.xlsx + bug fixes for Optimization_Stats.xlsx: - Lots of logic added to initializeTabuStats() method in ExcelExport to process the individual changes between all the Schedules when they're optimized all together with the full list of TimeSlots - Fixed some logic in updateLeagueStats() for Optimization_Stats.xlsx that wasn't updating the quality of Schedules properly after the second optimization round -Changed TabuList to allow for the ArrayList<Move> of Tabu moves to be passed and used for processing Tabu Moves in the combined schedule optimization - Extra logic added to League main() --> will be removed in next commit along with a lot of other redundant and left-over code
Signed-off-by: Brady Norton <bnort.11@gmail.com>
</commit_message>
<xml_diff>
--- a/Optimization_Stats.xlsx
+++ b/Optimization_Stats.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="41">
   <si>
     <t>Schedule (Pre-Optimization)</t>
   </si>
@@ -29,15 +29,24 @@
     <t>Total TimeSlots</t>
   </si>
   <si>
-    <t>Used TimeSlots</t>
-  </si>
-  <si>
     <t>Unused TimeSlots</t>
   </si>
   <si>
+    <t>TimeSlot Usage %</t>
+  </si>
+  <si>
     <t>Scheduling Success %</t>
   </si>
   <si>
+    <t>Teams</t>
+  </si>
+  <si>
+    <t>Games per Team</t>
+  </si>
+  <si>
+    <t>Quality</t>
+  </si>
+  <si>
     <t>Division U7 (Tier: 1)</t>
   </si>
   <si>
@@ -101,13 +110,31 @@
     <t>84.09%</t>
   </si>
   <si>
-    <t>87.5%</t>
+    <t>77.27%</t>
+  </si>
+  <si>
+    <t>85.23%</t>
+  </si>
+  <si>
+    <t>88.64%</t>
   </si>
   <si>
     <t>100.0%</t>
   </si>
   <si>
-    <t>84.85%</t>
+    <t>45.45%</t>
+  </si>
+  <si>
+    <t>95.45%</t>
+  </si>
+  <si>
+    <t>70.45%</t>
+  </si>
+  <si>
+    <t>Optimization Time</t>
+  </si>
+  <si>
+    <t>0 min, 49 sec</t>
   </si>
 </sst>
 </file>
@@ -168,7 +195,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -182,6 +209,9 @@
     <col min="6" max="6" width="20.0" customWidth="true"/>
     <col min="7" max="7" width="20.0" customWidth="true"/>
     <col min="8" max="8" width="20.0" customWidth="true"/>
+    <col min="9" max="9" width="20.0" customWidth="true"/>
+    <col min="10" max="10" width="20.0" customWidth="true"/>
+    <col min="11" max="11" width="20.0" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -209,10 +239,19 @@
       <c r="H1" t="s" s="2">
         <v>7</v>
       </c>
+      <c r="I1" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="1">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B2" t="n" s="1">
         <v>44.0</v>
@@ -227,18 +266,27 @@
         <v>44.0</v>
       </c>
       <c r="F2" t="n" s="1">
-        <v>33.0</v>
-      </c>
-      <c r="G2" t="n" s="1">
         <v>11.0</v>
       </c>
+      <c r="G2" t="s" s="1">
+        <v>12</v>
+      </c>
       <c r="H2" t="s" s="1">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="I2" t="n" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J2" t="n" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="K2" t="n" s="1">
+        <v>146.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B3" t="n" s="1">
         <v>44.0</v>
@@ -253,18 +301,27 @@
         <v>44.0</v>
       </c>
       <c r="F3" t="n" s="1">
-        <v>33.0</v>
-      </c>
-      <c r="G3" t="n" s="1">
         <v>11.0</v>
       </c>
+      <c r="G3" t="s" s="1">
+        <v>12</v>
+      </c>
       <c r="H3" t="s" s="1">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="I3" t="n" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J3" t="n" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="K3" t="n" s="1">
+        <v>144.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="1">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B4" t="n" s="1">
         <v>88.0</v>
@@ -279,18 +336,27 @@
         <v>88.0</v>
       </c>
       <c r="F4" t="n" s="1">
-        <v>72.0</v>
-      </c>
-      <c r="G4" t="n" s="1">
         <v>16.0</v>
       </c>
+      <c r="G4" t="s" s="1">
+        <v>15</v>
+      </c>
       <c r="H4" t="s" s="1">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="I4" t="n" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="J4" t="n" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="K4" t="n" s="1">
+        <v>157.55</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="1">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B5" t="n" s="1">
         <v>22.0</v>
@@ -305,18 +371,27 @@
         <v>22.0</v>
       </c>
       <c r="F5" t="n" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="G5" t="n" s="1">
         <v>7.0</v>
       </c>
+      <c r="G5" t="s" s="1">
+        <v>17</v>
+      </c>
       <c r="H5" t="s" s="1">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="I5" t="n" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J5" t="n" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="K5" t="n" s="1">
+        <v>134.45</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="1">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B6" t="n" s="1">
         <v>22.0</v>
@@ -331,18 +406,27 @@
         <v>22.0</v>
       </c>
       <c r="F6" t="n" s="1">
-        <v>9.0</v>
-      </c>
-      <c r="G6" t="n" s="1">
         <v>13.0</v>
       </c>
+      <c r="G6" t="s" s="1">
+        <v>19</v>
+      </c>
       <c r="H6" t="s" s="1">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="I6" t="n" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J6" t="n" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="K6" t="n" s="1">
+        <v>255.27</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="1">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B7" t="n" s="1">
         <v>44.0</v>
@@ -357,18 +441,27 @@
         <v>44.0</v>
       </c>
       <c r="F7" t="n" s="1">
-        <v>28.0</v>
-      </c>
-      <c r="G7" t="n" s="1">
         <v>16.0</v>
       </c>
+      <c r="G7" t="s" s="1">
+        <v>21</v>
+      </c>
       <c r="H7" t="s" s="1">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="I7" t="n" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="J7" t="n" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="K7" t="n" s="1">
+        <v>193.09</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="1">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B8" t="n" s="1">
         <v>44.0</v>
@@ -383,18 +476,27 @@
         <v>44.0</v>
       </c>
       <c r="F8" t="n" s="1">
-        <v>35.0</v>
-      </c>
-      <c r="G8" t="n" s="1">
         <v>9.0</v>
       </c>
+      <c r="G8" t="s" s="1">
+        <v>23</v>
+      </c>
       <c r="H8" t="s" s="1">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="I8" t="n" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="J8" t="n" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="K8" t="n" s="1">
+        <v>102.36</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="1">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B9" t="n" s="1">
         <v>22.0</v>
@@ -409,18 +511,27 @@
         <v>22.0</v>
       </c>
       <c r="F9" t="n" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="G9" t="n" s="1">
         <v>7.0</v>
       </c>
+      <c r="G9" t="s" s="1">
+        <v>17</v>
+      </c>
       <c r="H9" t="s" s="1">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="I9" t="n" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="J9" t="n" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="K9" t="n" s="1">
+        <v>138.45</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="1">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B10" t="n" s="1">
         <v>44.0</v>
@@ -435,18 +546,27 @@
         <v>44.0</v>
       </c>
       <c r="F10" t="n" s="1">
-        <v>32.0</v>
-      </c>
-      <c r="G10" t="n" s="1">
         <v>12.0</v>
       </c>
+      <c r="G10" t="s" s="1">
+        <v>26</v>
+      </c>
       <c r="H10" t="s" s="1">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="I10" t="n" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="J10" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K10" t="n" s="1">
+        <v>134.82</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="1">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B11" t="n" s="1">
         <v>44.0</v>
@@ -461,18 +581,27 @@
         <v>44.0</v>
       </c>
       <c r="F11" t="n" s="1">
-        <v>32.0</v>
-      </c>
-      <c r="G11" t="n" s="1">
         <v>12.0</v>
       </c>
+      <c r="G11" t="s" s="1">
+        <v>26</v>
+      </c>
       <c r="H11" t="s" s="1">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="I11" t="n" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J11" t="n" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="K11" t="n" s="1">
+        <v>158.82</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="1">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B12" t="n" s="1">
         <v>132.0</v>
@@ -487,18 +616,27 @@
         <v>132.0</v>
       </c>
       <c r="F12" t="n" s="1">
-        <v>89.0</v>
-      </c>
-      <c r="G12" t="n" s="1">
         <v>43.0</v>
       </c>
+      <c r="G12" t="s" s="1">
+        <v>29</v>
+      </c>
       <c r="H12" t="s" s="1">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="I12" t="n" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="J12" t="n" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="K12" t="n" s="1">
+        <v>374.73</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s" s="2">
         <v>1</v>
@@ -521,10 +659,19 @@
       <c r="H15" t="s" s="2">
         <v>7</v>
       </c>
+      <c r="I15" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="J15" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="K15" t="s" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="1">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B16" t="n" s="1">
         <v>44.0</v>
@@ -539,70 +686,97 @@
         <v>44.0</v>
       </c>
       <c r="F16" t="n" s="1">
-        <v>36.0</v>
-      </c>
-      <c r="G16" t="n" s="1">
         <v>8.0</v>
       </c>
+      <c r="G16" t="s" s="1">
+        <v>15</v>
+      </c>
       <c r="H16" t="s" s="1">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="I16" t="n" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J16" t="n" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="K16" t="n" s="1">
+        <v>100.55</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B17" t="n" s="1">
         <v>44.0</v>
       </c>
       <c r="C17" t="n" s="1">
-        <v>37.0</v>
+        <v>36.0</v>
       </c>
       <c r="D17" t="n" s="1">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="E17" t="n" s="1">
         <v>44.0</v>
       </c>
       <c r="F17" t="n" s="1">
-        <v>35.0</v>
-      </c>
-      <c r="G17" t="n" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="G17" t="s" s="1">
+        <v>32</v>
+      </c>
+      <c r="H17" t="s" s="1">
+        <v>15</v>
+      </c>
+      <c r="I17" t="n" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J17" t="n" s="1">
         <v>9.0</v>
       </c>
-      <c r="H17" t="s" s="1">
-        <v>28</v>
+      <c r="K17" t="n" s="1">
+        <v>117.18</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="1">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B18" t="n" s="1">
         <v>88.0</v>
       </c>
       <c r="C18" t="n" s="1">
-        <v>77.0</v>
+        <v>78.0</v>
       </c>
       <c r="D18" t="n" s="1">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="E18" t="n" s="1">
         <v>88.0</v>
       </c>
       <c r="F18" t="n" s="1">
-        <v>75.0</v>
-      </c>
-      <c r="G18" t="n" s="1">
         <v>13.0</v>
       </c>
+      <c r="G18" t="s" s="1">
+        <v>33</v>
+      </c>
       <c r="H18" t="s" s="1">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="I18" t="n" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="J18" t="n" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="K18" t="n" s="1">
+        <v>105.32</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="1">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B19" t="n" s="1">
         <v>22.0</v>
@@ -617,44 +791,62 @@
         <v>22.0</v>
       </c>
       <c r="F19" t="n" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="G19" t="n" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="G19" t="s" s="1">
+        <v>26</v>
+      </c>
+      <c r="H19" t="s" s="1">
+        <v>35</v>
+      </c>
+      <c r="I19" t="n" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J19" t="n" s="1">
         <v>7.0</v>
       </c>
-      <c r="H19" t="s" s="1">
-        <v>30</v>
+      <c r="K19" t="n" s="1">
+        <v>88.82</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="1">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B20" t="n" s="1">
         <v>22.0</v>
       </c>
       <c r="C20" t="n" s="1">
-        <v>22.0</v>
+        <v>21.0</v>
       </c>
       <c r="D20" t="n" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E20" t="n" s="1">
         <v>22.0</v>
       </c>
       <c r="F20" t="n" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="G20" t="n" s="1">
         <v>12.0</v>
       </c>
+      <c r="G20" t="s" s="1">
+        <v>36</v>
+      </c>
       <c r="H20" t="s" s="1">
-        <v>30</v>
+        <v>37</v>
+      </c>
+      <c r="I20" t="n" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="J20" t="n" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="K20" t="n" s="1">
+        <v>163.64</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="1">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B21" t="n" s="1">
         <v>44.0</v>
@@ -669,18 +861,27 @@
         <v>44.0</v>
       </c>
       <c r="F21" t="n" s="1">
-        <v>34.0</v>
-      </c>
-      <c r="G21" t="n" s="1">
-        <v>10.0</v>
+        <v>13.0</v>
+      </c>
+      <c r="G21" t="s" s="1">
+        <v>38</v>
       </c>
       <c r="H21" t="s" s="1">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="I21" t="n" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="J21" t="n" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="K21" t="n" s="1">
+        <v>113.64</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="1">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B22" t="n" s="1">
         <v>44.0</v>
@@ -695,18 +896,27 @@
         <v>44.0</v>
       </c>
       <c r="F22" t="n" s="1">
-        <v>35.0</v>
-      </c>
-      <c r="G22" t="n" s="1">
-        <v>9.0</v>
+        <v>8.0</v>
+      </c>
+      <c r="G22" t="s" s="1">
+        <v>15</v>
       </c>
       <c r="H22" t="s" s="1">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="I22" t="n" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="J22" t="n" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="K22" t="n" s="1">
+        <v>79.55</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="1">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B23" t="n" s="1">
         <v>22.0</v>
@@ -721,18 +931,27 @@
         <v>22.0</v>
       </c>
       <c r="F23" t="n" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="G23" t="n" s="1">
-        <v>7.0</v>
+        <v>5.0</v>
+      </c>
+      <c r="G23" t="s" s="1">
+        <v>32</v>
       </c>
       <c r="H23" t="s" s="1">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="I23" t="n" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="J23" t="n" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="K23" t="n" s="1">
+        <v>92.18</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="1">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B24" t="n" s="1">
         <v>44.0</v>
@@ -747,65 +966,102 @@
         <v>44.0</v>
       </c>
       <c r="F24" t="n" s="1">
-        <v>33.0</v>
-      </c>
-      <c r="G24" t="n" s="1">
         <v>11.0</v>
       </c>
+      <c r="G24" t="s" s="1">
+        <v>12</v>
+      </c>
       <c r="H24" t="s" s="1">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="I24" t="n" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="J24" t="n" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="K24" t="n" s="1">
+        <v>100.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="1">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B25" t="n" s="1">
         <v>44.0</v>
       </c>
       <c r="C25" t="n" s="1">
-        <v>36.0</v>
+        <v>37.0</v>
       </c>
       <c r="D25" t="n" s="1">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="E25" t="n" s="1">
         <v>44.0</v>
       </c>
       <c r="F25" t="n" s="1">
-        <v>34.0</v>
-      </c>
-      <c r="G25" t="n" s="1">
-        <v>10.0</v>
+        <v>11.0</v>
+      </c>
+      <c r="G25" t="s" s="1">
+        <v>12</v>
       </c>
       <c r="H25" t="s" s="1">
-        <v>12</v>
+        <v>31</v>
+      </c>
+      <c r="I25" t="n" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="J25" t="n" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="K25" t="n" s="1">
+        <v>119.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="1">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B26" t="n" s="1">
         <v>132.0</v>
       </c>
       <c r="C26" t="n" s="1">
-        <v>112.0</v>
+        <v>111.0</v>
       </c>
       <c r="D26" t="n" s="1">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
       <c r="E26" t="n" s="1">
         <v>132.0</v>
       </c>
       <c r="F26" t="n" s="1">
-        <v>97.0</v>
-      </c>
-      <c r="G26" t="n" s="1">
-        <v>35.0</v>
+        <v>39.0</v>
+      </c>
+      <c r="G26" t="s" s="1">
+        <v>38</v>
       </c>
       <c r="H26" t="s" s="1">
         <v>31</v>
+      </c>
+      <c r="I26" t="n" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="J26" t="n" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="K26" t="n" s="1">
+        <v>229.64</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="1">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug Fix & Clean-Up: - initializeTabuStats() method now properly summing and highlighting the proper range - Removed some unused code
Signed-off-by: Brady Norton <bnort.11@gmail.com>
</commit_message>
<xml_diff>
--- a/Optimization_Stats.xlsx
+++ b/Optimization_Stats.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="40">
   <si>
     <t>Schedule (Pre-Optimization)</t>
   </si>
@@ -107,13 +107,10 @@
     <t>Schedule (Post-Optimization)</t>
   </si>
   <si>
-    <t>84.09%</t>
-  </si>
-  <si>
     <t>77.27%</t>
   </si>
   <si>
-    <t>85.23%</t>
+    <t>82.95%</t>
   </si>
   <si>
     <t>88.64%</t>
@@ -122,19 +119,19 @@
     <t>100.0%</t>
   </si>
   <si>
-    <t>45.45%</t>
-  </si>
-  <si>
-    <t>95.45%</t>
-  </si>
-  <si>
-    <t>70.45%</t>
+    <t>50.0%</t>
+  </si>
+  <si>
+    <t>71.21%</t>
+  </si>
+  <si>
+    <t>86.36%</t>
   </si>
   <si>
     <t>Optimization Time</t>
   </si>
   <si>
-    <t>0 min, 49 sec</t>
+    <t>62 min, 2 sec</t>
   </si>
 </sst>
 </file>
@@ -677,10 +674,10 @@
         <v>44.0</v>
       </c>
       <c r="C16" t="n" s="1">
-        <v>37.0</v>
+        <v>36.0</v>
       </c>
       <c r="D16" t="n" s="1">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="E16" t="n" s="1">
         <v>44.0</v>
@@ -692,7 +689,7 @@
         <v>15</v>
       </c>
       <c r="H16" t="s" s="1">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="I16" t="n" s="1">
         <v>4.0</v>
@@ -701,7 +698,7 @@
         <v>9.0</v>
       </c>
       <c r="K16" t="n" s="1">
-        <v>100.55</v>
+        <v>108.55</v>
       </c>
     </row>
     <row r="17">
@@ -724,7 +721,7 @@
         <v>10.0</v>
       </c>
       <c r="G17" t="s" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H17" t="s" s="1">
         <v>15</v>
@@ -736,7 +733,7 @@
         <v>9.0</v>
       </c>
       <c r="K17" t="n" s="1">
-        <v>117.18</v>
+        <v>120.18</v>
       </c>
     </row>
     <row r="18">
@@ -756,14 +753,14 @@
         <v>88.0</v>
       </c>
       <c r="F18" t="n" s="1">
-        <v>13.0</v>
+        <v>15.0</v>
       </c>
       <c r="G18" t="s" s="1">
+        <v>32</v>
+      </c>
+      <c r="H18" t="s" s="1">
         <v>33</v>
       </c>
-      <c r="H18" t="s" s="1">
-        <v>34</v>
-      </c>
       <c r="I18" t="n" s="1">
         <v>8.0</v>
       </c>
@@ -771,7 +768,7 @@
         <v>9.0</v>
       </c>
       <c r="K18" t="n" s="1">
-        <v>105.32</v>
+        <v>112.14</v>
       </c>
     </row>
     <row r="19">
@@ -791,13 +788,13 @@
         <v>22.0</v>
       </c>
       <c r="F19" t="n" s="1">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="G19" t="s" s="1">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="H19" t="s" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I19" t="n" s="1">
         <v>3.0</v>
@@ -806,7 +803,7 @@
         <v>7.0</v>
       </c>
       <c r="K19" t="n" s="1">
-        <v>88.82</v>
+        <v>102.45</v>
       </c>
     </row>
     <row r="20">
@@ -817,22 +814,22 @@
         <v>22.0</v>
       </c>
       <c r="C20" t="n" s="1">
-        <v>21.0</v>
+        <v>22.0</v>
       </c>
       <c r="D20" t="n" s="1">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E20" t="n" s="1">
         <v>22.0</v>
       </c>
       <c r="F20" t="n" s="1">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="G20" t="s" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H20" t="s" s="1">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I20" t="n" s="1">
         <v>3.0</v>
@@ -841,7 +838,7 @@
         <v>7.0</v>
       </c>
       <c r="K20" t="n" s="1">
-        <v>163.64</v>
+        <v>157.0</v>
       </c>
     </row>
     <row r="21">
@@ -861,13 +858,13 @@
         <v>44.0</v>
       </c>
       <c r="F21" t="n" s="1">
-        <v>13.0</v>
+        <v>9.0</v>
       </c>
       <c r="G21" t="s" s="1">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="H21" t="s" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I21" t="n" s="1">
         <v>5.0</v>
@@ -876,7 +873,7 @@
         <v>8.0</v>
       </c>
       <c r="K21" t="n" s="1">
-        <v>113.64</v>
+        <v>86.36</v>
       </c>
     </row>
     <row r="22">
@@ -896,13 +893,13 @@
         <v>44.0</v>
       </c>
       <c r="F22" t="n" s="1">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="G22" t="s" s="1">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="H22" t="s" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I22" t="n" s="1">
         <v>5.0</v>
@@ -911,7 +908,7 @@
         <v>8.0</v>
       </c>
       <c r="K22" t="n" s="1">
-        <v>79.55</v>
+        <v>86.36</v>
       </c>
     </row>
     <row r="23">
@@ -931,10 +928,10 @@
         <v>22.0</v>
       </c>
       <c r="F23" t="n" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="G23" t="s" s="1">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="H23" t="s" s="1">
         <v>15</v>
@@ -946,7 +943,7 @@
         <v>9.0</v>
       </c>
       <c r="K23" t="n" s="1">
-        <v>92.18</v>
+        <v>119.45</v>
       </c>
     </row>
     <row r="24">
@@ -966,13 +963,13 @@
         <v>44.0</v>
       </c>
       <c r="F24" t="n" s="1">
-        <v>11.0</v>
+        <v>9.0</v>
       </c>
       <c r="G24" t="s" s="1">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H24" t="s" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I24" t="n" s="1">
         <v>5.0</v>
@@ -981,7 +978,7 @@
         <v>8.0</v>
       </c>
       <c r="K24" t="n" s="1">
-        <v>100.0</v>
+        <v>86.36</v>
       </c>
     </row>
     <row r="25">
@@ -992,22 +989,22 @@
         <v>44.0</v>
       </c>
       <c r="C25" t="n" s="1">
-        <v>37.0</v>
+        <v>36.0</v>
       </c>
       <c r="D25" t="n" s="1">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="E25" t="n" s="1">
         <v>44.0</v>
       </c>
       <c r="F25" t="n" s="1">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="G25" t="s" s="1">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="H25" t="s" s="1">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="I25" t="n" s="1">
         <v>4.0</v>
@@ -1016,7 +1013,7 @@
         <v>9.0</v>
       </c>
       <c r="K25" t="n" s="1">
-        <v>119.0</v>
+        <v>119.18</v>
       </c>
     </row>
     <row r="26">
@@ -1027,22 +1024,22 @@
         <v>132.0</v>
       </c>
       <c r="C26" t="n" s="1">
-        <v>111.0</v>
+        <v>114.0</v>
       </c>
       <c r="D26" t="n" s="1">
-        <v>21.0</v>
+        <v>18.0</v>
       </c>
       <c r="E26" t="n" s="1">
         <v>132.0</v>
       </c>
       <c r="F26" t="n" s="1">
-        <v>39.0</v>
+        <v>38.0</v>
       </c>
       <c r="G26" t="s" s="1">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H26" t="s" s="1">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="I26" t="n" s="1">
         <v>12.0</v>
@@ -1051,17 +1048,17 @@
         <v>9.0</v>
       </c>
       <c r="K26" t="n" s="1">
-        <v>229.64</v>
+        <v>203.36</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>